<commit_message>
Various changes to figure out mass balance
</commit_message>
<xml_diff>
--- a/Matlab/P. putida/Carbon Balance.xlsx
+++ b/Matlab/P. putida/Carbon Balance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365coloradoedu-my.sharepoint.com/personal/jefo6893_colorado_edu/Documents/Projects/Annie Thompson/Git Repository/Matlab/P. putida/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{9AD4AB57-E492-DA49-98AE-F60371075EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91D700ED-53D2-4E4B-A6B2-35F809CD4E25}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{9AD4AB57-E492-DA49-98AE-F60371075EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3F360FF-AB62-0846-829F-2F6FD1C7DD5D}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="12860" windowHeight="16100" activeTab="2" xr2:uid="{BDD80896-4C14-014B-A1B8-A0585B58D2AC}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="12860" windowHeight="16100" xr2:uid="{BDD80896-4C14-014B-A1B8-A0585B58D2AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -513,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3506D80-295E-8340-91DC-34C52D3C32DC}">
-  <dimension ref="C3:I14"/>
+  <dimension ref="C3:K14"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -535,8 +535,8 @@
     <col min="21" max="21" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="3:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D4" s="1">
         <v>5.0159337830000004</v>
       </c>
@@ -552,8 +552,12 @@
       <c r="H4" s="1">
         <v>42.973611730000002</v>
       </c>
-    </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="K4">
+        <f>190*8</f>
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" x14ac:dyDescent="0.2">
       <c r="D5">
         <f>D4*10</f>
         <v>50.159337830000005</v>
@@ -579,8 +583,8 @@
         <v>1602.88573563</v>
       </c>
     </row>
-    <row r="7" spans="3:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="3:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>10</v>
       </c>
@@ -601,7 +605,7 @@
       </c>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:11" x14ac:dyDescent="0.2">
       <c r="D9">
         <f>D8*10</f>
         <v>8.527000000000001</v>
@@ -627,7 +631,7 @@
         <v>910.11774000000003</v>
       </c>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:11" x14ac:dyDescent="0.2">
       <c r="H10" t="s">
         <v>9</v>
       </c>
@@ -635,7 +639,7 @@
         <v>1117.0999999999999</v>
       </c>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:11" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
         <v>1</v>
       </c>
@@ -643,7 +647,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:11" x14ac:dyDescent="0.2">
       <c r="E13">
         <v>500</v>
       </c>
@@ -651,7 +655,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:11" x14ac:dyDescent="0.2">
       <c r="E14">
         <f>E13*3</f>
         <v>1500</v>
@@ -2691,7 +2695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAED7E14-C0F6-D44B-B42B-7F79240B54B2}">
   <dimension ref="A1:D348"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>